<commit_message>
documentation and benchmarks revised
</commit_message>
<xml_diff>
--- a/benches/results/benchmark-results.xlsx
+++ b/benches/results/benchmark-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\uarikan\repos\orx\orx-parallel\benches\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAAF2F8-4DED-49CD-B70A-FD1D88058FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A20EC54-8274-4EF6-8C44-56BE4F5024F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25905" yWindow="-1950" windowWidth="26010" windowHeight="20985" activeTab="2" xr2:uid="{23836B73-0E02-4EF4-9D35-18409F12CF45}"/>
+    <workbookView xWindow="-25905" yWindow="-1950" windowWidth="26010" windowHeight="20985" activeTab="3" xr2:uid="{23836B73-0E02-4EF4-9D35-18409F12CF45}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="242">
   <si>
     <t>computation</t>
   </si>
@@ -705,6 +705,90 @@
   </si>
   <si>
     <t>**6.63 (0.21)**</t>
+  </si>
+  <si>
+    <t>collect_iter_into_par.rs</t>
+  </si>
+  <si>
+    <t>48.09 (1.00)</t>
+  </si>
+  <si>
+    <t>59.54 (1.24)</t>
+  </si>
+  <si>
+    <t>16.84 (0.35)</t>
+  </si>
+  <si>
+    <t>**16.21 (0.34)**</t>
+  </si>
+  <si>
+    <t>`inputs.iter().iter_into_par().map(map).filter(filter).collect()`</t>
+  </si>
+  <si>
+    <t>reduce_iter_into_par.rs</t>
+  </si>
+  <si>
+    <t>`inputs.iter_into_par().map(map).filter(filter).reduce(reduce)`</t>
+  </si>
+  <si>
+    <t>8.69 (1.00)</t>
+  </si>
+  <si>
+    <t>57.64 (6.63)</t>
+  </si>
+  <si>
+    <t>2.85 (0.33)</t>
+  </si>
+  <si>
+    <t>33.07 (1.00)</t>
+  </si>
+  <si>
+    <t>213.36 (6.45)</t>
+  </si>
+  <si>
+    <t>7.53 (0.23)</t>
+  </si>
+  <si>
+    <t>**7.53 (0.23)**</t>
+  </si>
+  <si>
+    <t>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce_iter_into_par.rs)</t>
+  </si>
+  <si>
+    <t>find_iter_into_par.rs</t>
+  </si>
+  <si>
+    <t>`inputs.into_iter().iter_into_par().map(map).filter(filter).find(&amp;find)`</t>
+  </si>
+  <si>
+    <t>39.17 (1.00)</t>
+  </si>
+  <si>
+    <t>54.83 (1.40)</t>
+  </si>
+  <si>
+    <t>11.95 (0.30)</t>
+  </si>
+  <si>
+    <t>44.53 (1.00)</t>
+  </si>
+  <si>
+    <t>55.31 (1.24)</t>
+  </si>
+  <si>
+    <t>11.78 (0.26)</t>
+  </si>
+  <si>
+    <t>41.22 (1.00)</t>
+  </si>
+  <si>
+    <t>50.59 (1.23)</t>
+  </si>
+  <si>
+    <t>11.47 (0.28)</t>
+  </si>
+  <si>
+    <t>**11.78 (0.26)**</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C658BCA-0CAA-4A56-A9CF-C42905156614}">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38:K46"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51:K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,11 +1263,11 @@
         <v>2.4662999999999999</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I39" si="0">IF(E3="","",TEXT(E3, "0.00")&amp;" (1.00)")</f>
+        <f t="shared" ref="I3:I43" si="0">IF(E3="","",TEXT(E3, "0.00")&amp;" (1.00)")</f>
         <v>5.92 (1.00)</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:L40" si="1">IF(F3="","",TEXT(F3,"0.00")&amp;" ("&amp;TEXT(F3/$E3,"0.00")&amp;")")</f>
+        <f t="shared" ref="J3:L44" si="1">IF(F3="","",TEXT(F3,"0.00")&amp;" ("&amp;TEXT(F3/$E3,"0.00")&amp;")")</f>
         <v>12.58 (2.12)</v>
       </c>
       <c r="K3" s="1" t="str">
@@ -1510,11 +1594,11 @@
         <v>9.00 (1.00)</v>
       </c>
       <c r="J12" s="1" t="str">
-        <f t="shared" ref="J12:J39" si="2">IF(F12="","",TEXT(F12,"0.00")&amp;" ("&amp;TEXT(F12/$E12,"0.00")&amp;")")</f>
+        <f t="shared" ref="J12:J43" si="2">IF(F12="","",TEXT(F12,"0.00")&amp;" ("&amp;TEXT(F12/$E12,"0.00")&amp;")")</f>
         <v>5.17 (0.57)</v>
       </c>
       <c r="K12" s="1" t="str">
-        <f t="shared" ref="K12:K39" si="3">IF(G12="","",TEXT(G12,"0.00")&amp;" ("&amp;TEXT(G12/$E12,"0.00")&amp;")")</f>
+        <f t="shared" ref="K12:K43" si="3">IF(G12="","",TEXT(G12,"0.00")&amp;" ("&amp;TEXT(G12/$E12,"0.00")&amp;")")</f>
         <v>2.56 (0.28)</v>
       </c>
       <c r="L12" s="1" t="str">
@@ -1555,44 +1639,43 @@
         <v>6.99 (0.19)</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>55</v>
-      </c>
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
+        <v>214</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="D14" s="1">
         <v>65536</v>
       </c>
       <c r="E14" s="2">
-        <v>2.6233</v>
+        <v>10.97</v>
       </c>
       <c r="F14" s="2">
-        <v>10.317</v>
+        <v>19.260000000000002</v>
       </c>
       <c r="G14" s="2">
-        <v>1.3491</v>
-      </c>
-      <c r="H14" s="2"/>
+        <v>3.54</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3.6</v>
+      </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2.62 (1.00)</v>
+        <v>10.97 (1.00)</v>
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>10.32 (3.93)</v>
+        <v>19.26 (1.76)</v>
       </c>
       <c r="K14" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>1.35 (0.51)</v>
+        <v>3.54 (0.32)</v>
       </c>
       <c r="L14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>3.60 (0.33)</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1600,63 +1683,68 @@
         <v>262144</v>
       </c>
       <c r="E15" s="2">
-        <v>12.673</v>
+        <v>48.09</v>
       </c>
       <c r="F15" s="2">
-        <v>8.9997000000000007</v>
+        <v>59.54</v>
       </c>
       <c r="G15" s="2">
-        <v>3.601</v>
-      </c>
-      <c r="H15" s="2"/>
+        <v>16.84</v>
+      </c>
+      <c r="H15" s="2">
+        <v>16.21</v>
+      </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>12.67 (1.00)</v>
+        <v>48.09 (1.00)</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9.00 (0.71)</v>
+        <v>59.54 (1.24)</v>
       </c>
       <c r="K15" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>3.60 (0.28)</v>
+        <v>16.84 (0.35)</v>
       </c>
       <c r="L15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>16.21 (0.34)</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1">
         <v>65536</v>
       </c>
       <c r="E16" s="2">
-        <v>50.262999999999998</v>
+        <v>2.6233</v>
       </c>
       <c r="F16" s="2">
-        <v>33.634</v>
+        <v>10.317</v>
       </c>
       <c r="G16" s="2">
-        <v>10.427</v>
+        <v>1.3491</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>50.26 (1.00)</v>
+        <v>2.62 (1.00)</v>
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>33.63 (0.67)</v>
+        <v>10.32 (3.93)</v>
       </c>
       <c r="K16" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>10.43 (0.21)</v>
+        <v>1.35 (0.51)</v>
       </c>
       <c r="L16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1668,26 +1756,26 @@
         <v>262144</v>
       </c>
       <c r="E17" s="2">
-        <v>217.07</v>
+        <v>12.673</v>
       </c>
       <c r="F17" s="2">
-        <v>146.77000000000001</v>
+        <v>8.9997000000000007</v>
       </c>
       <c r="G17" s="2">
-        <v>39.869</v>
+        <v>3.601</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>217.07 (1.00)</v>
+        <v>12.67 (1.00)</v>
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>146.77 (0.68)</v>
+        <v>9.00 (0.71)</v>
       </c>
       <c r="K17" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>39.87 (0.18)</v>
+        <v>3.60 (0.28)</v>
       </c>
       <c r="L17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1696,35 +1784,35 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1">
         <v>65536</v>
       </c>
       <c r="E18" s="2">
-        <v>10.840999999999999</v>
+        <v>50.262999999999998</v>
       </c>
       <c r="F18" s="2">
-        <v>2.8065000000000002</v>
+        <v>33.634</v>
       </c>
       <c r="G18" s="2">
-        <v>2.9670000000000001</v>
+        <v>10.427</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>10.84 (1.00)</v>
+        <v>50.26 (1.00)</v>
       </c>
       <c r="J18" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2.81 (0.26)</v>
+        <v>33.63 (0.67)</v>
       </c>
       <c r="K18" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>2.97 (0.27)</v>
+        <v>10.43 (0.21)</v>
       </c>
       <c r="L18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1736,26 +1824,26 @@
         <v>262144</v>
       </c>
       <c r="E19" s="2">
-        <v>51.540999999999997</v>
+        <v>217.07</v>
       </c>
       <c r="F19" s="2">
-        <v>9.7356999999999996</v>
+        <v>146.77000000000001</v>
       </c>
       <c r="G19" s="2">
-        <v>9.0901999999999994</v>
+        <v>39.869</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>51.54 (1.00)</v>
+        <v>217.07 (1.00)</v>
       </c>
       <c r="J19" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9.74 (0.19)</v>
+        <v>146.77 (0.68)</v>
       </c>
       <c r="K19" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>9.09 (0.18)</v>
+        <v>39.87 (0.18)</v>
       </c>
       <c r="L19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1764,35 +1852,35 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1">
         <v>65536</v>
       </c>
       <c r="E20" s="2">
-        <v>7.0456000000000003</v>
+        <v>10.840999999999999</v>
       </c>
       <c r="F20" s="2">
-        <v>1.8204</v>
+        <v>2.8065000000000002</v>
       </c>
       <c r="G20" s="2">
-        <v>2.3199999999999998</v>
+        <v>2.9670000000000001</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>7.05 (1.00)</v>
+        <v>10.84 (1.00)</v>
       </c>
       <c r="J20" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1.82 (0.26)</v>
+        <v>2.81 (0.26)</v>
       </c>
       <c r="K20" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>2.32 (0.33)</v>
+        <v>2.97 (0.27)</v>
       </c>
       <c r="L20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1804,26 +1892,26 @@
         <v>262144</v>
       </c>
       <c r="E21" s="2">
-        <v>30.954999999999998</v>
+        <v>51.540999999999997</v>
       </c>
       <c r="F21" s="2">
-        <v>5.4555999999999996</v>
+        <v>9.7356999999999996</v>
       </c>
       <c r="G21" s="2">
-        <v>6.4320000000000004</v>
+        <v>9.0901999999999994</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>30.96 (1.00)</v>
+        <v>51.54 (1.00)</v>
       </c>
       <c r="J21" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5.46 (0.18)</v>
+        <v>9.74 (0.19)</v>
       </c>
       <c r="K21" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6.43 (0.21)</v>
+        <v>9.09 (0.18)</v>
       </c>
       <c r="L21" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1832,35 +1920,35 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D22" s="1">
         <v>65536</v>
       </c>
       <c r="E22" s="2">
-        <v>6.57</v>
+        <v>7.0456000000000003</v>
       </c>
       <c r="F22" s="2">
-        <v>4.0922000000000001</v>
+        <v>1.8204</v>
       </c>
       <c r="G22" s="2">
-        <v>2.1758000000000002</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>6.57 (1.00)</v>
+        <v>7.05 (1.00)</v>
       </c>
       <c r="J22" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4.09 (0.62)</v>
+        <v>1.82 (0.26)</v>
       </c>
       <c r="K22" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>2.18 (0.33)</v>
+        <v>2.32 (0.33)</v>
       </c>
       <c r="L22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1872,26 +1960,26 @@
         <v>262144</v>
       </c>
       <c r="E23" s="2">
-        <v>31.92</v>
+        <v>30.954999999999998</v>
       </c>
       <c r="F23" s="2">
-        <v>16.157</v>
+        <v>5.4555999999999996</v>
       </c>
       <c r="G23" s="2">
-        <v>7.0662000000000003</v>
+        <v>6.4320000000000004</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>31.92 (1.00)</v>
+        <v>30.96 (1.00)</v>
       </c>
       <c r="J23" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>16.16 (0.51)</v>
+        <v>5.46 (0.18)</v>
       </c>
       <c r="K23" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>7.07 (0.22)</v>
+        <v>6.43 (0.21)</v>
       </c>
       <c r="L23" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1900,35 +1988,35 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1">
         <v>65536</v>
       </c>
       <c r="E24" s="2">
-        <v>7.3449999999999998</v>
+        <v>6.57</v>
       </c>
       <c r="F24" s="2">
-        <v>3.4548999999999999</v>
+        <v>4.0922000000000001</v>
       </c>
       <c r="G24" s="2">
-        <v>2.3349000000000002</v>
+        <v>2.1758000000000002</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>7.35 (1.00)</v>
+        <v>6.57 (1.00)</v>
       </c>
       <c r="J24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3.45 (0.47)</v>
+        <v>4.09 (0.62)</v>
       </c>
       <c r="K24" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>2.33 (0.32)</v>
+        <v>2.18 (0.33)</v>
       </c>
       <c r="L24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1940,26 +2028,26 @@
         <v>262144</v>
       </c>
       <c r="E25" s="2">
-        <v>32.256999999999998</v>
+        <v>31.92</v>
       </c>
       <c r="F25" s="2">
-        <v>7.8517999999999999</v>
+        <v>16.157</v>
       </c>
       <c r="G25" s="2">
-        <v>6.9630999999999998</v>
+        <v>7.0662000000000003</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>32.26 (1.00)</v>
+        <v>31.92 (1.00)</v>
       </c>
       <c r="J25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7.85 (0.24)</v>
+        <v>16.16 (0.51)</v>
       </c>
       <c r="K25" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6.96 (0.22)</v>
+        <v>7.07 (0.22)</v>
       </c>
       <c r="L25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1968,35 +2056,35 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" s="1">
         <v>65536</v>
       </c>
       <c r="E26" s="2">
-        <v>0.42070999999999997</v>
+        <v>7.3449999999999998</v>
       </c>
       <c r="F26" s="2">
-        <v>8.3529999999999998</v>
+        <v>3.4548999999999999</v>
       </c>
       <c r="G26" s="2">
-        <v>0.47410000000000002</v>
+        <v>2.3349000000000002</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.42 (1.00)</v>
+        <v>7.35 (1.00)</v>
       </c>
       <c r="J26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8.35 (19.85)</v>
+        <v>3.45 (0.47)</v>
       </c>
       <c r="K26" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0.47 (1.13)</v>
+        <v>2.33 (0.32)</v>
       </c>
       <c r="L26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2008,26 +2096,26 @@
         <v>262144</v>
       </c>
       <c r="E27" s="2">
-        <v>1.9987999999999999</v>
+        <v>32.256999999999998</v>
       </c>
       <c r="F27" s="2">
-        <v>12.180999999999999</v>
+        <v>7.8517999999999999</v>
       </c>
       <c r="G27" s="2">
-        <v>1.0935999999999999</v>
+        <v>6.9630999999999998</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2.00 (1.00)</v>
+        <v>32.26 (1.00)</v>
       </c>
       <c r="J27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12.18 (6.09)</v>
+        <v>7.85 (0.24)</v>
       </c>
       <c r="K27" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>1.09 (0.55)</v>
+        <v>6.96 (0.22)</v>
       </c>
       <c r="L27" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2036,35 +2124,35 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D28" s="1">
         <v>65536</v>
       </c>
       <c r="E28" s="2">
-        <v>2.7408000000000001</v>
+        <v>0.42070999999999997</v>
       </c>
       <c r="F28" s="2">
-        <v>8.4231999999999996</v>
+        <v>8.3529999999999998</v>
       </c>
       <c r="G28" s="2">
-        <v>1.3303</v>
+        <v>0.47410000000000002</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2.74 (1.00)</v>
+        <v>0.42 (1.00)</v>
       </c>
       <c r="J28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8.42 (3.07)</v>
+        <v>8.35 (19.85)</v>
       </c>
       <c r="K28" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>1.33 (0.49)</v>
+        <v>0.47 (1.13)</v>
       </c>
       <c r="L28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2076,26 +2164,26 @@
         <v>262144</v>
       </c>
       <c r="E29" s="2">
-        <v>12.398</v>
+        <v>1.9987999999999999</v>
       </c>
       <c r="F29" s="2">
-        <v>4.6563999999999997</v>
+        <v>12.180999999999999</v>
       </c>
       <c r="G29" s="2">
-        <v>2.8759000000000001</v>
+        <v>1.0935999999999999</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>12.40 (1.00)</v>
+        <v>2.00 (1.00)</v>
       </c>
       <c r="J29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4.66 (0.38)</v>
+        <v>12.18 (6.09)</v>
       </c>
       <c r="K29" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>2.88 (0.23)</v>
+        <v>1.09 (0.55)</v>
       </c>
       <c r="L29" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2104,35 +2192,35 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="1">
         <v>65536</v>
       </c>
       <c r="E30" s="2">
-        <v>28.831</v>
+        <v>2.7408000000000001</v>
       </c>
       <c r="F30" s="2">
-        <v>33.415999999999997</v>
+        <v>8.4231999999999996</v>
       </c>
       <c r="G30" s="2">
-        <v>6.5812999999999997</v>
+        <v>1.3303</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>28.83 (1.00)</v>
+        <v>2.74 (1.00)</v>
       </c>
       <c r="J30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>33.42 (1.16)</v>
+        <v>8.42 (3.07)</v>
       </c>
       <c r="K30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6.58 (0.23)</v>
+        <v>1.33 (0.49)</v>
       </c>
       <c r="L30" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2144,26 +2232,26 @@
         <v>262144</v>
       </c>
       <c r="E31" s="2">
-        <v>123.5</v>
+        <v>12.398</v>
       </c>
       <c r="F31" s="2">
-        <v>56.485999999999997</v>
+        <v>4.6563999999999997</v>
       </c>
       <c r="G31" s="2">
-        <v>21.157</v>
+        <v>2.8759000000000001</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>123.50 (1.00)</v>
+        <v>12.40 (1.00)</v>
       </c>
       <c r="J31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>56.49 (0.46)</v>
+        <v>4.66 (0.38)</v>
       </c>
       <c r="K31" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>21.16 (0.17)</v>
+        <v>2.88 (0.23)</v>
       </c>
       <c r="L31" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2172,35 +2260,35 @@
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D32" s="1">
         <v>65536</v>
       </c>
       <c r="E32" s="2">
-        <v>1.5598000000000001</v>
+        <v>28.831</v>
       </c>
       <c r="F32" s="2">
-        <v>8.5344999999999995</v>
+        <v>33.415999999999997</v>
       </c>
       <c r="G32" s="2">
-        <v>0.82877000000000001</v>
+        <v>6.5812999999999997</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1.56 (1.00)</v>
+        <v>28.83 (1.00)</v>
       </c>
       <c r="J32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8.53 (5.47)</v>
+        <v>33.42 (1.16)</v>
       </c>
       <c r="K32" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0.83 (0.53)</v>
+        <v>6.58 (0.23)</v>
       </c>
       <c r="L32" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2212,26 +2300,26 @@
         <v>262144</v>
       </c>
       <c r="E33" s="2">
-        <v>6.2243000000000004</v>
+        <v>123.5</v>
       </c>
       <c r="F33" s="2">
-        <v>4.5681000000000003</v>
+        <v>56.485999999999997</v>
       </c>
       <c r="G33" s="2">
-        <v>1.8440000000000001</v>
+        <v>21.157</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>6.22 (1.00)</v>
+        <v>123.50 (1.00)</v>
       </c>
       <c r="J33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4.57 (0.73)</v>
+        <v>56.49 (0.46)</v>
       </c>
       <c r="K33" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>1.84 (0.30)</v>
+        <v>21.16 (0.17)</v>
       </c>
       <c r="L33" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2240,35 +2328,35 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D34" s="1">
         <v>65536</v>
       </c>
       <c r="E34" s="2">
-        <v>3.4589999999999998E-3</v>
+        <v>1.5598000000000001</v>
       </c>
       <c r="F34" s="2">
-        <v>8.1609999999999996</v>
+        <v>8.5344999999999995</v>
       </c>
       <c r="G34" s="2">
-        <v>0.18029000000000001</v>
+        <v>0.82877000000000001</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.00 (1.00)</v>
+        <v>1.56 (1.00)</v>
       </c>
       <c r="J34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8.16 (2359.35)</v>
+        <v>8.53 (5.47)</v>
       </c>
       <c r="K34" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0.18 (52.12)</v>
+        <v>0.83 (0.53)</v>
       </c>
       <c r="L34" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2280,26 +2368,26 @@
         <v>262144</v>
       </c>
       <c r="E35" s="2">
-        <v>1.524E-3</v>
+        <v>6.2243000000000004</v>
       </c>
       <c r="F35" s="2">
-        <v>9.8289000000000009</v>
+        <v>4.5681000000000003</v>
       </c>
       <c r="G35" s="2">
-        <v>0.20765</v>
+        <v>1.8440000000000001</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.00 (1.00)</v>
+        <v>6.22 (1.00)</v>
       </c>
       <c r="J35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9.83 (6449.41)</v>
+        <v>4.57 (0.73)</v>
       </c>
       <c r="K35" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0.21 (136.25)</v>
+        <v>1.84 (0.30)</v>
       </c>
       <c r="L35" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2308,35 +2396,35 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1">
         <v>65536</v>
       </c>
       <c r="E36" s="2">
-        <v>7.2176</v>
+        <v>3.4589999999999998E-3</v>
       </c>
       <c r="F36" s="2">
-        <v>4.4261999999999997</v>
+        <v>8.1609999999999996</v>
       </c>
       <c r="G36" s="2">
-        <v>2.3797000000000001</v>
+        <v>0.18029000000000001</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>7.22 (1.00)</v>
+        <v>0.00 (1.00)</v>
       </c>
       <c r="J36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4.43 (0.61)</v>
+        <v>8.16 (2359.35)</v>
       </c>
       <c r="K36" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>2.38 (0.33)</v>
+        <v>0.18 (52.12)</v>
       </c>
       <c r="L36" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2348,26 +2436,26 @@
         <v>262144</v>
       </c>
       <c r="E37" s="2">
-        <v>32.281999999999996</v>
+        <v>1.524E-3</v>
       </c>
       <c r="F37" s="2">
-        <v>8.9908000000000001</v>
+        <v>9.8289000000000009</v>
       </c>
       <c r="G37" s="2">
-        <v>6.6261999999999999</v>
+        <v>0.20765</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>32.28 (1.00)</v>
+        <v>0.00 (1.00)</v>
       </c>
       <c r="J37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>8.99 (0.28)</v>
+        <v>9.83 (6449.41)</v>
       </c>
       <c r="K37" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>6.63 (0.21)</v>
+        <v>0.21 (136.25)</v>
       </c>
       <c r="L37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2375,39 +2463,36 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>54</v>
-      </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
+      </c>
+      <c r="D38" s="1">
+        <v>65536</v>
       </c>
       <c r="E38" s="2">
-        <v>153.02000000000001</v>
+        <v>7.2176</v>
       </c>
       <c r="F38" s="2">
-        <v>101.62</v>
+        <v>4.4261999999999997</v>
       </c>
       <c r="G38" s="2">
-        <v>30.07</v>
+        <v>2.3797000000000001</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>153.02 (1.00)</v>
+        <v>7.22 (1.00)</v>
       </c>
       <c r="J38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>101.62 (0.66)</v>
+        <v>4.43 (0.61)</v>
       </c>
       <c r="K38" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>30.07 (0.20)</v>
+        <v>2.38 (0.33)</v>
       </c>
       <c r="L38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2415,262 +2500,497 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D39" s="1" t="s">
-        <v>28</v>
+      <c r="D39" s="1">
+        <v>262144</v>
       </c>
       <c r="E39" s="2">
-        <v>170.8</v>
+        <v>32.281999999999996</v>
       </c>
       <c r="F39" s="2">
-        <v>120.63</v>
+        <v>8.9908000000000001</v>
       </c>
       <c r="G39" s="2">
-        <v>27.529</v>
+        <v>6.6261999999999999</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>170.80 (1.00)</v>
+        <v>32.28 (1.00)</v>
       </c>
       <c r="J39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>120.63 (0.71)</v>
+        <v>8.99 (0.28)</v>
       </c>
       <c r="K39" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>27.53 (0.16)</v>
+        <v>6.63 (0.21)</v>
       </c>
       <c r="L39" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D40" s="1" t="s">
-        <v>29</v>
+    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" s="1">
+        <v>65536</v>
       </c>
       <c r="E40" s="2">
-        <v>170.99</v>
+        <v>8.6881000000000004</v>
       </c>
       <c r="F40" s="2">
-        <v>108.14</v>
+        <v>57.640999999999998</v>
       </c>
       <c r="G40" s="2">
-        <v>29.541</v>
+        <v>2.8466999999999998</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="1" t="str">
-        <f t="shared" ref="I40:I46" si="4">IF(E40="","",TEXT(E40, "0.00")&amp;" (1.00)")</f>
-        <v>170.99 (1.00)</v>
+        <f t="shared" ref="I40:I41" si="4">IF(E40="","",TEXT(E40, "0.00")&amp;" (1.00)")</f>
+        <v>8.69 (1.00)</v>
       </c>
       <c r="J40" s="1" t="str">
-        <f t="shared" ref="J40:J46" si="5">IF(F40="","",TEXT(F40,"0.00")&amp;" ("&amp;TEXT(F40/$E40,"0.00")&amp;")")</f>
-        <v>108.14 (0.63)</v>
+        <f t="shared" ref="J40:J41" si="5">IF(F40="","",TEXT(F40,"0.00")&amp;" ("&amp;TEXT(F40/$E40,"0.00")&amp;")")</f>
+        <v>57.64 (6.63)</v>
       </c>
       <c r="K40" s="1" t="str">
-        <f t="shared" ref="K40:L46" si="6">IF(G40="","",TEXT(G40,"0.00")&amp;" ("&amp;TEXT(G40/$E40,"0.00")&amp;")")</f>
-        <v>29.54 (0.17)</v>
+        <f t="shared" ref="K40:K41" si="6">IF(G40="","",TEXT(G40,"0.00")&amp;" ("&amp;TEXT(G40/$E40,"0.00")&amp;")")</f>
+        <v>2.85 (0.33)</v>
       </c>
       <c r="L40" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="L40:L41" si="7">IF(H40="","",TEXT(H40,"0.00")&amp;" ("&amp;TEXT(H40/$E40,"0.00")&amp;")")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>27</v>
+      <c r="D41" s="1">
+        <v>262144</v>
       </c>
       <c r="E41" s="2">
-        <v>39.222999999999999</v>
+        <v>33.066000000000003</v>
       </c>
       <c r="F41" s="2">
-        <v>11.346</v>
+        <v>213.36</v>
       </c>
       <c r="G41" s="2">
-        <v>8.6453000000000007</v>
+        <v>7.5279999999999996</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>39.22 (1.00)</v>
+        <v>33.07 (1.00)</v>
       </c>
       <c r="J41" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>11.35 (0.29)</v>
+        <v>213.36 (6.45)</v>
       </c>
       <c r="K41" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>8.65 (0.22)</v>
+        <v>7.53 (0.23)</v>
       </c>
       <c r="L41" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
       <c r="D42" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E42" s="2">
-        <v>46.274999999999999</v>
+        <v>153.02000000000001</v>
       </c>
       <c r="F42" s="2">
-        <v>11.959</v>
+        <v>101.62</v>
       </c>
       <c r="G42" s="2">
-        <v>9.67</v>
+        <v>30.07</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>46.28 (1.00)</v>
+        <f t="shared" si="0"/>
+        <v>153.02 (1.00)</v>
       </c>
       <c r="J42" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>11.96 (0.26)</v>
+        <f t="shared" si="2"/>
+        <v>101.62 (0.66)</v>
       </c>
       <c r="K42" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>9.67 (0.21)</v>
+        <f t="shared" si="3"/>
+        <v>30.07 (0.20)</v>
       </c>
       <c r="L42" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D43" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E43" s="2">
-        <v>40.976999999999997</v>
+        <v>170.8</v>
       </c>
       <c r="F43" s="2">
-        <v>7.9154999999999998</v>
+        <v>120.63</v>
       </c>
       <c r="G43" s="2">
-        <v>8</v>
+        <v>27.529</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>40.98 (1.00)</v>
+        <f t="shared" si="0"/>
+        <v>170.80 (1.00)</v>
       </c>
       <c r="J43" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>7.92 (0.19)</v>
+        <f t="shared" si="2"/>
+        <v>120.63 (0.71)</v>
       </c>
       <c r="K43" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>8.00 (0.20)</v>
+        <f t="shared" si="3"/>
+        <v>27.53 (0.16)</v>
       </c>
       <c r="L43" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" t="s">
-        <v>33</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E44" s="2">
-        <v>2.4849000000000001</v>
+        <v>170.99</v>
       </c>
       <c r="F44" s="2">
-        <v>8.2228999999999992</v>
+        <v>108.14</v>
       </c>
       <c r="G44" s="2">
-        <v>1.1926000000000001</v>
+        <v>29.541</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>2.48 (1.00)</v>
+        <f t="shared" ref="I44:I53" si="8">IF(E44="","",TEXT(E44, "0.00")&amp;" (1.00)")</f>
+        <v>170.99 (1.00)</v>
       </c>
       <c r="J44" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>8.22 (3.31)</v>
+        <f t="shared" ref="J44:J53" si="9">IF(F44="","",TEXT(F44,"0.00")&amp;" ("&amp;TEXT(F44/$E44,"0.00")&amp;")")</f>
+        <v>108.14 (0.63)</v>
       </c>
       <c r="K44" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>1.19 (0.48)</v>
+        <f t="shared" ref="K44:L53" si="10">IF(G44="","",TEXT(G44,"0.00")&amp;" ("&amp;TEXT(G44/$E44,"0.00")&amp;")")</f>
+        <v>29.54 (0.17)</v>
       </c>
       <c r="L44" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
       <c r="D45" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E45" s="2">
-        <v>2.5051000000000001</v>
+        <v>39.222999999999999</v>
       </c>
       <c r="F45" s="2">
-        <v>12.153</v>
+        <v>11.346</v>
       </c>
       <c r="G45" s="2">
-        <v>1.2394000000000001</v>
+        <v>8.6453000000000007</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>2.51 (1.00)</v>
+        <f t="shared" si="8"/>
+        <v>39.22 (1.00)</v>
       </c>
       <c r="J45" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>12.15 (4.85)</v>
+        <f t="shared" si="9"/>
+        <v>11.35 (0.29)</v>
       </c>
       <c r="K45" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>1.24 (0.49)</v>
+        <f t="shared" si="10"/>
+        <v>8.65 (0.22)</v>
       </c>
       <c r="L45" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D46" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E46" s="2">
-        <v>2.6457999999999999</v>
+        <v>46.274999999999999</v>
       </c>
       <c r="F46" s="2">
-        <v>12.824999999999999</v>
+        <v>11.959</v>
       </c>
       <c r="G46" s="2">
-        <v>1.2027000000000001</v>
+        <v>9.67</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
+        <v>46.28 (1.00)</v>
+      </c>
+      <c r="J46" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>11.96 (0.26)</v>
+      </c>
+      <c r="K46" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>9.67 (0.21)</v>
+      </c>
+      <c r="L46" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="2">
+        <v>40.976999999999997</v>
+      </c>
+      <c r="F47" s="2">
+        <v>7.9154999999999998</v>
+      </c>
+      <c r="G47" s="2">
+        <v>8</v>
+      </c>
+      <c r="H47" s="2"/>
+      <c r="I47" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>40.98 (1.00)</v>
+      </c>
+      <c r="J47" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>7.92 (0.19)</v>
+      </c>
+      <c r="K47" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>8.00 (0.20)</v>
+      </c>
+      <c r="L47" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="2">
+        <v>2.4849000000000001</v>
+      </c>
+      <c r="F48" s="2">
+        <v>8.2228999999999992</v>
+      </c>
+      <c r="G48" s="2">
+        <v>1.1926000000000001</v>
+      </c>
+      <c r="H48" s="2"/>
+      <c r="I48" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>2.48 (1.00)</v>
+      </c>
+      <c r="J48" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>8.22 (3.31)</v>
+      </c>
+      <c r="K48" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1.19 (0.48)</v>
+      </c>
+      <c r="L48" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2.5051000000000001</v>
+      </c>
+      <c r="F49" s="2">
+        <v>12.153</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1.2394000000000001</v>
+      </c>
+      <c r="H49" s="2"/>
+      <c r="I49" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>2.51 (1.00)</v>
+      </c>
+      <c r="J49" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>12.15 (4.85)</v>
+      </c>
+      <c r="K49" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>1.24 (0.49)</v>
+      </c>
+      <c r="L49" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="2">
+        <v>2.6457999999999999</v>
+      </c>
+      <c r="F50" s="2">
+        <v>12.824999999999999</v>
+      </c>
+      <c r="G50" s="2">
+        <v>1.2027000000000001</v>
+      </c>
+      <c r="H50" s="2"/>
+      <c r="I50" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>2.65 (1.00)</v>
       </c>
-      <c r="J46" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="J50" s="1" t="str">
+        <f t="shared" si="9"/>
         <v>12.83 (4.85)</v>
       </c>
-      <c r="K46" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="K50" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>1.20 (0.45)</v>
       </c>
-      <c r="L46" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="L50" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>230</v>
+      </c>
+      <c r="C51" t="s">
+        <v>231</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="2">
+        <v>39.171999999999997</v>
+      </c>
+      <c r="F51" s="2">
+        <v>54.83</v>
+      </c>
+      <c r="G51" s="2">
+        <v>11.946</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>39.17 (1.00)</v>
+      </c>
+      <c r="J51" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>54.83 (1.40)</v>
+      </c>
+      <c r="K51" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>11.95 (0.30)</v>
+      </c>
+      <c r="L51" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="2">
+        <v>44.533000000000001</v>
+      </c>
+      <c r="F52" s="2">
+        <v>55.308</v>
+      </c>
+      <c r="G52" s="2">
+        <v>11.776999999999999</v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>44.53 (1.00)</v>
+      </c>
+      <c r="J52" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>55.31 (1.24)</v>
+      </c>
+      <c r="K52" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>11.78 (0.26)</v>
+      </c>
+      <c r="L52" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D53" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="2">
+        <v>41.22</v>
+      </c>
+      <c r="F53" s="2">
+        <v>50.587000000000003</v>
+      </c>
+      <c r="G53" s="2">
+        <v>11.467000000000001</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>41.22 (1.00)</v>
+      </c>
+      <c r="J53" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>50.59 (1.23)</v>
+      </c>
+      <c r="K53" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>11.47 (0.28)</v>
+      </c>
+      <c r="L53" s="1" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -2681,14 +3001,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD6D5CC-12E7-4025-9415-A12E1BCA77C3}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="7" width="15.5546875" customWidth="1"/>
@@ -2750,7 +3071,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B7" si="0">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A3&amp;")"</f>
+        <f t="shared" ref="B3:B8" si="0">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A3&amp;")"</f>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/collect_filtermap.rs)</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2769,7 +3090,7 @@
         <v>168</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I7" si="1">"**"&amp;G3&amp;"**"</f>
+        <f t="shared" ref="G3:I8" si="1">"**"&amp;G3&amp;"**"</f>
         <v>****6.37 (0.40)****</v>
       </c>
     </row>
@@ -2885,17 +3206,46 @@
         <v>****6.99 (0.19)****</v>
       </c>
     </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/collect_iter_into_par.rs)</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8" t="s">
+        <v>218</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>****16.21 (0.34)****</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FEBB30-DFE1-40ED-A94E-23FF3A0CBAA0}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3183,7 +3533,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D17" s="1">
         <v>262144</v>
       </c>
@@ -3197,7 +3547,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>43</v>
       </c>
@@ -3217,7 +3567,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D19" s="1">
         <v>262144</v>
       </c>
@@ -3231,7 +3581,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>44</v>
       </c>
@@ -3251,7 +3601,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D21" s="1">
         <v>262144</v>
       </c>
@@ -3265,7 +3615,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>46</v>
       </c>
@@ -3285,7 +3635,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D23" s="1">
         <v>262144</v>
       </c>
@@ -3298,8 +3648,23 @@
       <c r="G23" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>229</v>
+      </c>
+      <c r="K23" t="s">
+        <v>221</v>
+      </c>
+      <c r="L23" t="s">
+        <v>225</v>
+      </c>
+      <c r="M23" t="s">
+        <v>226</v>
+      </c>
+      <c r="N23" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>50</v>
       </c>
@@ -3319,7 +3684,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D25" s="1">
         <v>262144</v>
       </c>
@@ -3333,316 +3698,389 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D26" s="1">
+        <v>65536</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D27" s="1">
+        <v>262144</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>166</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>166</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" t="str">
-        <f>"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A30&amp;")"</f>
-        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/count_filtermap.rs)</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G30" t="str">
-        <f>"**"&amp;F30&amp;"**"</f>
-        <v>****3.60 (0.28)****</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" ref="B31:B41" si="0">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A31&amp;")"</f>
-        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/count_flatmap.rs)</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G31" t="str">
-        <f t="shared" ref="F31:G41" si="1">"**"&amp;F31&amp;"**"</f>
-        <v>****39.87 (0.18)****</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/count_map_filter.rs)</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G32" t="str">
-        <f t="shared" si="1"/>
-        <v>****9.09 (0.18)****</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/count_map.rs)</v>
+        <f>"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A33&amp;")"</f>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/count_filtermap.rs)</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>97</v>
+        <v>204</v>
+      </c>
+      <c r="G33" t="str">
+        <f>"**"&amp;F33&amp;"**"</f>
+        <v>****3.60 (0.28)****</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce_map_filter.rs)</v>
+        <f t="shared" ref="B34:B45" si="0">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A34&amp;")"</f>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/count_flatmap.rs)</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="1"/>
-        <v>****7.07 (0.22)****</v>
+        <f t="shared" ref="G34:G44" si="1">"**"&amp;F34&amp;"**"</f>
+        <v>****39.87 (0.18)****</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce_map.rs)</v>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/count_map_filter.rs)</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
-        <v>****6.96 (0.22)****</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>****9.09 (0.18)****</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce.rs)</v>
-      </c>
-      <c r="C36" t="s">
-        <v>39</v>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/count_map.rs)</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="1"/>
-        <v>****1.09 (0.55)****</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/sum_filtermap.rs)</v>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce_map_filter.rs)</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
-        <v>****2.88 (0.23)****</v>
+        <v>****7.07 (0.22)****</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce_map.rs)</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>****6.96 (0.22)****</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce.rs)</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>****1.09 (0.55)****</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/sum_filtermap.rs)</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>****2.88 (0.23)****</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>43</v>
       </c>
-      <c r="B38" t="str">
+      <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/sum_flatmap.rs)</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G38" t="str">
+      <c r="G41" t="str">
         <f t="shared" si="1"/>
         <v>****21.16 (0.17)****</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>44</v>
       </c>
-      <c r="B39" t="str">
+      <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/sum_map_filter.rs)</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G39" t="str">
+      <c r="G42" t="str">
         <f t="shared" si="1"/>
         <v>****1.84 (0.30)****</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B40" t="str">
+      <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/sum.rs)</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
-      <c r="B41" t="str">
+      <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce_long_chain.rs)</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G41" t="str">
+      <c r="G44" t="str">
         <f t="shared" si="1"/>
         <v>****6.63 (0.21)****</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/reduce_iter_into_par.rs)</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3654,13 +4092,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86143C3F-8878-42FB-956C-4C6FDD5D34D0}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
     <col min="3" max="3" width="34.88671875" customWidth="1"/>
     <col min="4" max="6" width="19.21875" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -3830,6 +4269,54 @@
         <v>197</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>166</v>
@@ -3880,7 +4367,7 @@
         <v>31</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" ref="B21:B22" si="0">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A21&amp;")"</f>
+        <f t="shared" ref="B21:B23" si="0">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A21&amp;")"</f>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/find_map_filter.rs)</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -3896,7 +4383,7 @@
         <v>202</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" ref="H21:H22" si="1">"**"&amp;F21&amp;"**"</f>
+        <f t="shared" ref="H21:H23" si="1">"**"&amp;F21&amp;"**"</f>
         <v>****9.67 (0.21)****</v>
       </c>
     </row>
@@ -3923,6 +4410,31 @@
       <c r="H22" t="str">
         <f t="shared" si="1"/>
         <v>****1.24 (0.49)****</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/find_iter_into_par.rs)</v>
+      </c>
+      <c r="C23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>****11.78 (0.26)****</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
parallel drain benchmark results are added
</commit_message>
<xml_diff>
--- a/benches/results/benchmark-results.xlsx
+++ b/benches/results/benchmark-results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\uarikan\repos\orx\orx-parallel\benches\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\uarikan\orx\orx-parallel\benches\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A20EC54-8274-4EF6-8C44-56BE4F5024F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39864CF-BBBA-497B-B826-4B1F4D0A5023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25905" yWindow="-1950" windowWidth="26010" windowHeight="20985" activeTab="3" xr2:uid="{23836B73-0E02-4EF4-9D35-18409F12CF45}"/>
+    <workbookView xWindow="-51705" yWindow="-1950" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{23836B73-0E02-4EF4-9D35-18409F12CF45}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="249">
   <si>
     <t>computation</t>
   </si>
@@ -789,6 +789,28 @@
   </si>
   <si>
     <t>**11.78 (0.26)**</t>
+  </si>
+  <si>
+    <t>drain_vec_collect_map_filter.rs</t>
+  </si>
+  <si>
+    <t>`inputs.par_drain()
+  .map(map).filter(filter).collect()`</t>
+  </si>
+  <si>
+    <t>`inputs.par_drain().map(map).filter(filter).collect()`</t>
+  </si>
+  <si>
+    <t>58.37 (1.00)</t>
+  </si>
+  <si>
+    <t>23.10 (0.40)</t>
+  </si>
+  <si>
+    <t>13.96 (0.24)</t>
+  </si>
+  <si>
+    <t>**12.84 (0.22)**</t>
   </si>
 </sst>
 </file>
@@ -1149,16 +1171,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C658BCA-0CAA-4A56-A9CF-C42905156614}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51:K53"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L11" sqref="I11:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="17.44140625" customWidth="1"/>
     <col min="8" max="8" width="23.5546875" bestFit="1" customWidth="1"/>
@@ -1263,11 +1285,11 @@
         <v>2.4662999999999999</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I43" si="0">IF(E3="","",TEXT(E3, "0.00")&amp;" (1.00)")</f>
+        <f t="shared" ref="I3:I45" si="0">IF(E3="","",TEXT(E3, "0.00")&amp;" (1.00)")</f>
         <v>5.92 (1.00)</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:L44" si="1">IF(F3="","",TEXT(F3,"0.00")&amp;" ("&amp;TEXT(F3/$E3,"0.00")&amp;")")</f>
+        <f t="shared" ref="J3:L46" si="1">IF(F3="","",TEXT(F3,"0.00")&amp;" ("&amp;TEXT(F3/$E3,"0.00")&amp;")")</f>
         <v>12.58 (2.12)</v>
       </c>
       <c r="K3" s="1" t="str">
@@ -1497,41 +1519,41 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>242</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="D10" s="1">
         <v>65536</v>
       </c>
       <c r="E10" s="2">
-        <v>8.8025000000000002</v>
+        <v>10.45</v>
       </c>
       <c r="F10" s="2">
-        <v>4.5034000000000001</v>
+        <v>12.68</v>
       </c>
       <c r="G10" s="2">
-        <v>3.3849999999999998</v>
+        <v>3.81</v>
       </c>
       <c r="H10" s="2">
-        <v>3.7915999999999999</v>
+        <v>4.12</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>8.80 (1.00)</v>
+        <f t="shared" ref="I10:I11" si="2">IF(E10="","",TEXT(E10, "0.00")&amp;" (1.00)")</f>
+        <v>10.45 (1.00)</v>
       </c>
       <c r="J10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>4.50 (0.51)</v>
+        <f t="shared" ref="J10:J11" si="3">IF(F10="","",TEXT(F10,"0.00")&amp;" ("&amp;TEXT(F10/$E10,"0.00")&amp;")")</f>
+        <v>12.68 (1.21)</v>
       </c>
       <c r="K10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>3.39 (0.38)</v>
+        <f t="shared" ref="K10:K11" si="4">IF(G10="","",TEXT(G10,"0.00")&amp;" ("&amp;TEXT(G10/$E10,"0.00")&amp;")")</f>
+        <v>3.81 (0.36)</v>
       </c>
       <c r="L10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>3.79 (0.43)</v>
+        <f t="shared" ref="L10:L11" si="5">IF(H10="","",TEXT(H10,"0.00")&amp;" ("&amp;TEXT(H10/$E10,"0.00")&amp;")")</f>
+        <v>4.12 (0.39)</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1539,71 +1561,71 @@
         <v>262144</v>
       </c>
       <c r="E11" s="2">
-        <v>36.21</v>
+        <v>58.37</v>
       </c>
       <c r="F11" s="2">
-        <v>14.364000000000001</v>
+        <v>23.1</v>
       </c>
       <c r="G11" s="2">
-        <v>11.760999999999999</v>
+        <v>13.96</v>
       </c>
       <c r="H11" s="2">
-        <v>14.465</v>
+        <v>12.84</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>36.21 (1.00)</v>
+        <f t="shared" si="2"/>
+        <v>58.37 (1.00)</v>
       </c>
       <c r="J11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>14.36 (0.40)</v>
+        <f t="shared" si="3"/>
+        <v>23.10 (0.40)</v>
       </c>
       <c r="K11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>11.76 (0.32)</v>
+        <f t="shared" si="4"/>
+        <v>13.96 (0.24)</v>
       </c>
       <c r="L11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>14.47 (0.40)</v>
+        <f t="shared" si="5"/>
+        <v>12.84 (0.22)</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1">
         <v>65536</v>
       </c>
       <c r="E12" s="2">
-        <v>9.0028000000000006</v>
+        <v>8.8025000000000002</v>
       </c>
       <c r="F12" s="2">
-        <v>5.17</v>
+        <v>4.5034000000000001</v>
       </c>
       <c r="G12" s="2">
-        <v>2.5619000000000001</v>
+        <v>3.3849999999999998</v>
       </c>
       <c r="H12" s="2">
-        <v>2.387</v>
+        <v>3.7915999999999999</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>9.00 (1.00)</v>
+        <v>8.80 (1.00)</v>
       </c>
       <c r="J12" s="1" t="str">
-        <f t="shared" ref="J12:J43" si="2">IF(F12="","",TEXT(F12,"0.00")&amp;" ("&amp;TEXT(F12/$E12,"0.00")&amp;")")</f>
-        <v>5.17 (0.57)</v>
+        <f t="shared" si="1"/>
+        <v>4.50 (0.51)</v>
       </c>
       <c r="K12" s="1" t="str">
-        <f t="shared" ref="K12:K43" si="3">IF(G12="","",TEXT(G12,"0.00")&amp;" ("&amp;TEXT(G12/$E12,"0.00")&amp;")")</f>
-        <v>2.56 (0.28)</v>
+        <f t="shared" si="1"/>
+        <v>3.39 (0.38)</v>
       </c>
       <c r="L12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2.39 (0.27)</v>
+        <v>3.79 (0.43)</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1611,71 +1633,71 @@
         <v>262144</v>
       </c>
       <c r="E13" s="2">
-        <v>35.886000000000003</v>
+        <v>36.21</v>
       </c>
       <c r="F13" s="2">
-        <v>10.106999999999999</v>
+        <v>14.364000000000001</v>
       </c>
       <c r="G13" s="2">
-        <v>7.3982000000000001</v>
+        <v>11.760999999999999</v>
       </c>
       <c r="H13" s="2">
-        <v>6.9901</v>
+        <v>14.465</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>35.89 (1.00)</v>
+        <v>36.21 (1.00)</v>
       </c>
       <c r="J13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>10.11 (0.28)</v>
+        <f t="shared" si="1"/>
+        <v>14.36 (0.40)</v>
       </c>
       <c r="K13" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>7.40 (0.21)</v>
+        <f t="shared" si="1"/>
+        <v>11.76 (0.32)</v>
       </c>
       <c r="L13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>6.99 (0.19)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>14.47 (0.40)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>214</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>219</v>
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
       </c>
       <c r="D14" s="1">
         <v>65536</v>
       </c>
       <c r="E14" s="2">
-        <v>10.97</v>
+        <v>9.0028000000000006</v>
       </c>
       <c r="F14" s="2">
-        <v>19.260000000000002</v>
+        <v>5.17</v>
       </c>
       <c r="G14" s="2">
-        <v>3.54</v>
+        <v>2.5619000000000001</v>
       </c>
       <c r="H14" s="2">
-        <v>3.6</v>
+        <v>2.387</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>10.97 (1.00)</v>
+        <v>9.00 (1.00)</v>
       </c>
       <c r="J14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>19.26 (1.76)</v>
+        <f t="shared" ref="J14:J45" si="6">IF(F14="","",TEXT(F14,"0.00")&amp;" ("&amp;TEXT(F14/$E14,"0.00")&amp;")")</f>
+        <v>5.17 (0.57)</v>
       </c>
       <c r="K14" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>3.54 (0.32)</v>
+        <f t="shared" ref="K14:K45" si="7">IF(G14="","",TEXT(G14,"0.00")&amp;" ("&amp;TEXT(G14/$E14,"0.00")&amp;")")</f>
+        <v>2.56 (0.28)</v>
       </c>
       <c r="L14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3.60 (0.33)</v>
+        <v>2.39 (0.27)</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1683,612 +1705,616 @@
         <v>262144</v>
       </c>
       <c r="E15" s="2">
-        <v>48.09</v>
+        <v>35.886000000000003</v>
       </c>
       <c r="F15" s="2">
-        <v>59.54</v>
+        <v>10.106999999999999</v>
       </c>
       <c r="G15" s="2">
-        <v>16.84</v>
+        <v>7.3982000000000001</v>
       </c>
       <c r="H15" s="2">
-        <v>16.21</v>
+        <v>6.9901</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>48.09 (1.00)</v>
+        <v>35.89 (1.00)</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>59.54 (1.24)</v>
+        <f t="shared" si="6"/>
+        <v>10.11 (0.28)</v>
       </c>
       <c r="K15" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>16.84 (0.35)</v>
+        <f t="shared" si="7"/>
+        <v>7.40 (0.21)</v>
       </c>
       <c r="L15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>16.21 (0.34)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
+        <v>6.99 (0.19)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
+        <v>214</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="D16" s="1">
         <v>65536</v>
       </c>
       <c r="E16" s="2">
-        <v>2.6233</v>
+        <v>10.97</v>
       </c>
       <c r="F16" s="2">
-        <v>10.317</v>
+        <v>19.260000000000002</v>
       </c>
       <c r="G16" s="2">
-        <v>1.3491</v>
-      </c>
-      <c r="H16" s="2"/>
+        <v>3.54</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3.6</v>
+      </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2.62 (1.00)</v>
+        <v>10.97 (1.00)</v>
       </c>
       <c r="J16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>10.32 (3.93)</v>
+        <f t="shared" si="6"/>
+        <v>19.26 (1.76)</v>
       </c>
       <c r="K16" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>1.35 (0.51)</v>
+        <f t="shared" si="7"/>
+        <v>3.54 (0.32)</v>
       </c>
       <c r="L16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+        <v>3.60 (0.33)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D17" s="1">
         <v>262144</v>
       </c>
       <c r="E17" s="2">
-        <v>12.673</v>
+        <v>48.09</v>
       </c>
       <c r="F17" s="2">
-        <v>8.9997000000000007</v>
+        <v>59.54</v>
       </c>
       <c r="G17" s="2">
-        <v>3.601</v>
-      </c>
-      <c r="H17" s="2"/>
+        <v>16.84</v>
+      </c>
+      <c r="H17" s="2">
+        <v>16.21</v>
+      </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>12.67 (1.00)</v>
+        <v>48.09 (1.00)</v>
       </c>
       <c r="J17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>9.00 (0.71)</v>
+        <f t="shared" si="6"/>
+        <v>59.54 (1.24)</v>
       </c>
       <c r="K17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>3.60 (0.28)</v>
+        <f t="shared" si="7"/>
+        <v>16.84 (0.35)</v>
       </c>
       <c r="L17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+        <v>16.21 (0.34)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1">
         <v>65536</v>
       </c>
       <c r="E18" s="2">
-        <v>50.262999999999998</v>
+        <v>2.6233</v>
       </c>
       <c r="F18" s="2">
-        <v>33.634</v>
+        <v>10.317</v>
       </c>
       <c r="G18" s="2">
-        <v>10.427</v>
+        <v>1.3491</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>50.26 (1.00)</v>
+        <v>2.62 (1.00)</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>33.63 (0.67)</v>
+        <f t="shared" si="6"/>
+        <v>10.32 (3.93)</v>
       </c>
       <c r="K18" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>10.43 (0.21)</v>
+        <f t="shared" si="7"/>
+        <v>1.35 (0.51)</v>
       </c>
       <c r="L18" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D19" s="1">
         <v>262144</v>
       </c>
       <c r="E19" s="2">
-        <v>217.07</v>
+        <v>12.673</v>
       </c>
       <c r="F19" s="2">
-        <v>146.77000000000001</v>
+        <v>8.9997000000000007</v>
       </c>
       <c r="G19" s="2">
-        <v>39.869</v>
+        <v>3.601</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>217.07 (1.00)</v>
+        <v>12.67 (1.00)</v>
       </c>
       <c r="J19" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>146.77 (0.68)</v>
+        <f t="shared" si="6"/>
+        <v>9.00 (0.71)</v>
       </c>
       <c r="K19" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>39.87 (0.18)</v>
+        <f t="shared" si="7"/>
+        <v>3.60 (0.28)</v>
       </c>
       <c r="L19" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1">
         <v>65536</v>
       </c>
       <c r="E20" s="2">
-        <v>10.840999999999999</v>
+        <v>50.262999999999998</v>
       </c>
       <c r="F20" s="2">
-        <v>2.8065000000000002</v>
+        <v>33.634</v>
       </c>
       <c r="G20" s="2">
-        <v>2.9670000000000001</v>
+        <v>10.427</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>10.84 (1.00)</v>
+        <v>50.26 (1.00)</v>
       </c>
       <c r="J20" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>2.81 (0.26)</v>
+        <f t="shared" si="6"/>
+        <v>33.63 (0.67)</v>
       </c>
       <c r="K20" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>2.97 (0.27)</v>
+        <f t="shared" si="7"/>
+        <v>10.43 (0.21)</v>
       </c>
       <c r="L20" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D21" s="1">
         <v>262144</v>
       </c>
       <c r="E21" s="2">
-        <v>51.540999999999997</v>
+        <v>217.07</v>
       </c>
       <c r="F21" s="2">
-        <v>9.7356999999999996</v>
+        <v>146.77000000000001</v>
       </c>
       <c r="G21" s="2">
-        <v>9.0901999999999994</v>
+        <v>39.869</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>51.54 (1.00)</v>
+        <v>217.07 (1.00)</v>
       </c>
       <c r="J21" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>9.74 (0.19)</v>
+        <f t="shared" si="6"/>
+        <v>146.77 (0.68)</v>
       </c>
       <c r="K21" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>9.09 (0.18)</v>
+        <f t="shared" si="7"/>
+        <v>39.87 (0.18)</v>
       </c>
       <c r="L21" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1">
         <v>65536</v>
       </c>
       <c r="E22" s="2">
-        <v>7.0456000000000003</v>
+        <v>10.840999999999999</v>
       </c>
       <c r="F22" s="2">
-        <v>1.8204</v>
+        <v>2.8065000000000002</v>
       </c>
       <c r="G22" s="2">
-        <v>2.3199999999999998</v>
+        <v>2.9670000000000001</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>7.05 (1.00)</v>
+        <v>10.84 (1.00)</v>
       </c>
       <c r="J22" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>1.82 (0.26)</v>
+        <f t="shared" si="6"/>
+        <v>2.81 (0.26)</v>
       </c>
       <c r="K22" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>2.32 (0.33)</v>
+        <f t="shared" si="7"/>
+        <v>2.97 (0.27)</v>
       </c>
       <c r="L22" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D23" s="1">
         <v>262144</v>
       </c>
       <c r="E23" s="2">
-        <v>30.954999999999998</v>
+        <v>51.540999999999997</v>
       </c>
       <c r="F23" s="2">
-        <v>5.4555999999999996</v>
+        <v>9.7356999999999996</v>
       </c>
       <c r="G23" s="2">
-        <v>6.4320000000000004</v>
+        <v>9.0901999999999994</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>30.96 (1.00)</v>
+        <v>51.54 (1.00)</v>
       </c>
       <c r="J23" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>5.46 (0.18)</v>
+        <f t="shared" si="6"/>
+        <v>9.74 (0.19)</v>
       </c>
       <c r="K23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>6.43 (0.21)</v>
+        <f t="shared" si="7"/>
+        <v>9.09 (0.18)</v>
       </c>
       <c r="L23" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D24" s="1">
         <v>65536</v>
       </c>
       <c r="E24" s="2">
-        <v>6.57</v>
+        <v>7.0456000000000003</v>
       </c>
       <c r="F24" s="2">
-        <v>4.0922000000000001</v>
+        <v>1.8204</v>
       </c>
       <c r="G24" s="2">
-        <v>2.1758000000000002</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>6.57 (1.00)</v>
+        <v>7.05 (1.00)</v>
       </c>
       <c r="J24" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>4.09 (0.62)</v>
+        <f t="shared" si="6"/>
+        <v>1.82 (0.26)</v>
       </c>
       <c r="K24" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>2.18 (0.33)</v>
+        <f t="shared" si="7"/>
+        <v>2.32 (0.33)</v>
       </c>
       <c r="L24" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D25" s="1">
         <v>262144</v>
       </c>
       <c r="E25" s="2">
-        <v>31.92</v>
+        <v>30.954999999999998</v>
       </c>
       <c r="F25" s="2">
-        <v>16.157</v>
+        <v>5.4555999999999996</v>
       </c>
       <c r="G25" s="2">
-        <v>7.0662000000000003</v>
+        <v>6.4320000000000004</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>31.92 (1.00)</v>
+        <v>30.96 (1.00)</v>
       </c>
       <c r="J25" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>16.16 (0.51)</v>
+        <f t="shared" si="6"/>
+        <v>5.46 (0.18)</v>
       </c>
       <c r="K25" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>7.07 (0.22)</v>
+        <f t="shared" si="7"/>
+        <v>6.43 (0.21)</v>
       </c>
       <c r="L25" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D26" s="1">
         <v>65536</v>
       </c>
       <c r="E26" s="2">
-        <v>7.3449999999999998</v>
+        <v>6.57</v>
       </c>
       <c r="F26" s="2">
-        <v>3.4548999999999999</v>
+        <v>4.0922000000000001</v>
       </c>
       <c r="G26" s="2">
-        <v>2.3349000000000002</v>
+        <v>2.1758000000000002</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>7.35 (1.00)</v>
+        <v>6.57 (1.00)</v>
       </c>
       <c r="J26" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>3.45 (0.47)</v>
+        <f t="shared" si="6"/>
+        <v>4.09 (0.62)</v>
       </c>
       <c r="K26" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>2.33 (0.32)</v>
+        <f t="shared" si="7"/>
+        <v>2.18 (0.33)</v>
       </c>
       <c r="L26" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D27" s="1">
         <v>262144</v>
       </c>
       <c r="E27" s="2">
-        <v>32.256999999999998</v>
+        <v>31.92</v>
       </c>
       <c r="F27" s="2">
-        <v>7.8517999999999999</v>
+        <v>16.157</v>
       </c>
       <c r="G27" s="2">
-        <v>6.9630999999999998</v>
+        <v>7.0662000000000003</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>32.26 (1.00)</v>
+        <v>31.92 (1.00)</v>
       </c>
       <c r="J27" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>7.85 (0.24)</v>
+        <f t="shared" si="6"/>
+        <v>16.16 (0.51)</v>
       </c>
       <c r="K27" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>6.96 (0.22)</v>
+        <f t="shared" si="7"/>
+        <v>7.07 (0.22)</v>
       </c>
       <c r="L27" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="1">
         <v>65536</v>
       </c>
       <c r="E28" s="2">
-        <v>0.42070999999999997</v>
+        <v>7.3449999999999998</v>
       </c>
       <c r="F28" s="2">
-        <v>8.3529999999999998</v>
+        <v>3.4548999999999999</v>
       </c>
       <c r="G28" s="2">
-        <v>0.47410000000000002</v>
+        <v>2.3349000000000002</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.42 (1.00)</v>
+        <v>7.35 (1.00)</v>
       </c>
       <c r="J28" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>8.35 (19.85)</v>
+        <f t="shared" si="6"/>
+        <v>3.45 (0.47)</v>
       </c>
       <c r="K28" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0.47 (1.13)</v>
+        <f t="shared" si="7"/>
+        <v>2.33 (0.32)</v>
       </c>
       <c r="L28" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D29" s="1">
         <v>262144</v>
       </c>
       <c r="E29" s="2">
-        <v>1.9987999999999999</v>
+        <v>32.256999999999998</v>
       </c>
       <c r="F29" s="2">
-        <v>12.180999999999999</v>
+        <v>7.8517999999999999</v>
       </c>
       <c r="G29" s="2">
-        <v>1.0935999999999999</v>
+        <v>6.9630999999999998</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2.00 (1.00)</v>
+        <v>32.26 (1.00)</v>
       </c>
       <c r="J29" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>12.18 (6.09)</v>
+        <f t="shared" si="6"/>
+        <v>7.85 (0.24)</v>
       </c>
       <c r="K29" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>1.09 (0.55)</v>
+        <f t="shared" si="7"/>
+        <v>6.96 (0.22)</v>
       </c>
       <c r="L29" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" s="1">
         <v>65536</v>
       </c>
       <c r="E30" s="2">
-        <v>2.7408000000000001</v>
+        <v>0.42070999999999997</v>
       </c>
       <c r="F30" s="2">
-        <v>8.4231999999999996</v>
+        <v>8.3529999999999998</v>
       </c>
       <c r="G30" s="2">
-        <v>1.3303</v>
+        <v>0.47410000000000002</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2.74 (1.00)</v>
+        <v>0.42 (1.00)</v>
       </c>
       <c r="J30" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>8.42 (3.07)</v>
+        <f t="shared" si="6"/>
+        <v>8.35 (19.85)</v>
       </c>
       <c r="K30" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>1.33 (0.49)</v>
+        <f t="shared" si="7"/>
+        <v>0.47 (1.13)</v>
       </c>
       <c r="L30" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D31" s="1">
         <v>262144</v>
       </c>
       <c r="E31" s="2">
-        <v>12.398</v>
+        <v>1.9987999999999999</v>
       </c>
       <c r="F31" s="2">
-        <v>4.6563999999999997</v>
+        <v>12.180999999999999</v>
       </c>
       <c r="G31" s="2">
-        <v>2.8759000000000001</v>
+        <v>1.0935999999999999</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>12.40 (1.00)</v>
+        <v>2.00 (1.00)</v>
       </c>
       <c r="J31" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>4.66 (0.38)</v>
+        <f t="shared" si="6"/>
+        <v>12.18 (6.09)</v>
       </c>
       <c r="K31" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>2.88 (0.23)</v>
+        <f t="shared" si="7"/>
+        <v>1.09 (0.55)</v>
       </c>
       <c r="L31" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" s="1">
         <v>65536</v>
       </c>
       <c r="E32" s="2">
-        <v>28.831</v>
+        <v>2.7408000000000001</v>
       </c>
       <c r="F32" s="2">
-        <v>33.415999999999997</v>
+        <v>8.4231999999999996</v>
       </c>
       <c r="G32" s="2">
-        <v>6.5812999999999997</v>
+        <v>1.3303</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>28.83 (1.00)</v>
+        <v>2.74 (1.00)</v>
       </c>
       <c r="J32" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>33.42 (1.16)</v>
+        <f t="shared" si="6"/>
+        <v>8.42 (3.07)</v>
       </c>
       <c r="K32" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>6.58 (0.23)</v>
+        <f t="shared" si="7"/>
+        <v>1.33 (0.49)</v>
       </c>
       <c r="L32" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2300,26 +2326,26 @@
         <v>262144</v>
       </c>
       <c r="E33" s="2">
-        <v>123.5</v>
+        <v>12.398</v>
       </c>
       <c r="F33" s="2">
-        <v>56.485999999999997</v>
+        <v>4.6563999999999997</v>
       </c>
       <c r="G33" s="2">
-        <v>21.157</v>
+        <v>2.8759000000000001</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>123.50 (1.00)</v>
+        <v>12.40 (1.00)</v>
       </c>
       <c r="J33" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>56.49 (0.46)</v>
+        <f t="shared" si="6"/>
+        <v>4.66 (0.38)</v>
       </c>
       <c r="K33" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>21.16 (0.17)</v>
+        <f t="shared" si="7"/>
+        <v>2.88 (0.23)</v>
       </c>
       <c r="L33" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2328,35 +2354,35 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1">
         <v>65536</v>
       </c>
       <c r="E34" s="2">
-        <v>1.5598000000000001</v>
+        <v>28.831</v>
       </c>
       <c r="F34" s="2">
-        <v>8.5344999999999995</v>
+        <v>33.415999999999997</v>
       </c>
       <c r="G34" s="2">
-        <v>0.82877000000000001</v>
+        <v>6.5812999999999997</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1.56 (1.00)</v>
+        <v>28.83 (1.00)</v>
       </c>
       <c r="J34" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>8.53 (5.47)</v>
+        <f t="shared" si="6"/>
+        <v>33.42 (1.16)</v>
       </c>
       <c r="K34" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0.83 (0.53)</v>
+        <f t="shared" si="7"/>
+        <v>6.58 (0.23)</v>
       </c>
       <c r="L34" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2368,26 +2394,26 @@
         <v>262144</v>
       </c>
       <c r="E35" s="2">
-        <v>6.2243000000000004</v>
+        <v>123.5</v>
       </c>
       <c r="F35" s="2">
-        <v>4.5681000000000003</v>
+        <v>56.485999999999997</v>
       </c>
       <c r="G35" s="2">
-        <v>1.8440000000000001</v>
+        <v>21.157</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>6.22 (1.00)</v>
+        <v>123.50 (1.00)</v>
       </c>
       <c r="J35" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>4.57 (0.73)</v>
+        <f t="shared" si="6"/>
+        <v>56.49 (0.46)</v>
       </c>
       <c r="K35" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>1.84 (0.30)</v>
+        <f t="shared" si="7"/>
+        <v>21.16 (0.17)</v>
       </c>
       <c r="L35" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2396,35 +2422,35 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D36" s="1">
         <v>65536</v>
       </c>
       <c r="E36" s="2">
-        <v>3.4589999999999998E-3</v>
+        <v>1.5598000000000001</v>
       </c>
       <c r="F36" s="2">
-        <v>8.1609999999999996</v>
+        <v>8.5344999999999995</v>
       </c>
       <c r="G36" s="2">
-        <v>0.18029000000000001</v>
+        <v>0.82877000000000001</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.00 (1.00)</v>
+        <v>1.56 (1.00)</v>
       </c>
       <c r="J36" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>8.16 (2359.35)</v>
+        <f t="shared" si="6"/>
+        <v>8.53 (5.47)</v>
       </c>
       <c r="K36" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0.18 (52.12)</v>
+        <f t="shared" si="7"/>
+        <v>0.83 (0.53)</v>
       </c>
       <c r="L36" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2436,26 +2462,26 @@
         <v>262144</v>
       </c>
       <c r="E37" s="2">
-        <v>1.524E-3</v>
+        <v>6.2243000000000004</v>
       </c>
       <c r="F37" s="2">
-        <v>9.8289000000000009</v>
+        <v>4.5681000000000003</v>
       </c>
       <c r="G37" s="2">
-        <v>0.20765</v>
+        <v>1.8440000000000001</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0.00 (1.00)</v>
+        <v>6.22 (1.00)</v>
       </c>
       <c r="J37" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>9.83 (6449.41)</v>
+        <f t="shared" si="6"/>
+        <v>4.57 (0.73)</v>
       </c>
       <c r="K37" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0.21 (136.25)</v>
+        <f t="shared" si="7"/>
+        <v>1.84 (0.30)</v>
       </c>
       <c r="L37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2464,35 +2490,35 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1">
         <v>65536</v>
       </c>
       <c r="E38" s="2">
-        <v>7.2176</v>
+        <v>3.4589999999999998E-3</v>
       </c>
       <c r="F38" s="2">
-        <v>4.4261999999999997</v>
+        <v>8.1609999999999996</v>
       </c>
       <c r="G38" s="2">
-        <v>2.3797000000000001</v>
+        <v>0.18029000000000001</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>7.22 (1.00)</v>
+        <v>0.00 (1.00)</v>
       </c>
       <c r="J38" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>4.43 (0.61)</v>
+        <f t="shared" si="6"/>
+        <v>8.16 (2359.35)</v>
       </c>
       <c r="K38" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>2.38 (0.33)</v>
+        <f t="shared" si="7"/>
+        <v>0.18 (52.12)</v>
       </c>
       <c r="L38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2504,66 +2530,66 @@
         <v>262144</v>
       </c>
       <c r="E39" s="2">
-        <v>32.281999999999996</v>
+        <v>1.524E-3</v>
       </c>
       <c r="F39" s="2">
-        <v>8.9908000000000001</v>
+        <v>9.8289000000000009</v>
       </c>
       <c r="G39" s="2">
-        <v>6.6261999999999999</v>
+        <v>0.20765</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>32.28 (1.00)</v>
+        <v>0.00 (1.00)</v>
       </c>
       <c r="J39" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>8.99 (0.28)</v>
+        <f t="shared" si="6"/>
+        <v>9.83 (6449.41)</v>
       </c>
       <c r="K39" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>6.63 (0.21)</v>
+        <f t="shared" si="7"/>
+        <v>0.21 (136.25)</v>
       </c>
       <c r="L39" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>220</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>221</v>
+        <v>50</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
       </c>
       <c r="D40" s="1">
         <v>65536</v>
       </c>
       <c r="E40" s="2">
-        <v>8.6881000000000004</v>
+        <v>7.2176</v>
       </c>
       <c r="F40" s="2">
-        <v>57.640999999999998</v>
+        <v>4.4261999999999997</v>
       </c>
       <c r="G40" s="2">
-        <v>2.8466999999999998</v>
+        <v>2.3797000000000001</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="1" t="str">
-        <f t="shared" ref="I40:I41" si="4">IF(E40="","",TEXT(E40, "0.00")&amp;" (1.00)")</f>
-        <v>8.69 (1.00)</v>
+        <f t="shared" si="0"/>
+        <v>7.22 (1.00)</v>
       </c>
       <c r="J40" s="1" t="str">
-        <f t="shared" ref="J40:J41" si="5">IF(F40="","",TEXT(F40,"0.00")&amp;" ("&amp;TEXT(F40/$E40,"0.00")&amp;")")</f>
-        <v>57.64 (6.63)</v>
+        <f t="shared" si="6"/>
+        <v>4.43 (0.61)</v>
       </c>
       <c r="K40" s="1" t="str">
-        <f t="shared" ref="K40:K41" si="6">IF(G40="","",TEXT(G40,"0.00")&amp;" ("&amp;TEXT(G40/$E40,"0.00")&amp;")")</f>
-        <v>2.85 (0.33)</v>
+        <f t="shared" si="7"/>
+        <v>2.38 (0.33)</v>
       </c>
       <c r="L40" s="1" t="str">
-        <f t="shared" ref="L40:L41" si="7">IF(H40="","",TEXT(H40,"0.00")&amp;" ("&amp;TEXT(H40/$E40,"0.00")&amp;")")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2572,128 +2598,134 @@
         <v>262144</v>
       </c>
       <c r="E41" s="2">
-        <v>33.066000000000003</v>
+        <v>32.281999999999996</v>
       </c>
       <c r="F41" s="2">
-        <v>213.36</v>
+        <v>8.9908000000000001</v>
       </c>
       <c r="G41" s="2">
-        <v>7.5279999999999996</v>
+        <v>6.6261999999999999</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>33.07 (1.00)</v>
+        <f t="shared" si="0"/>
+        <v>32.28 (1.00)</v>
       </c>
       <c r="J41" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>213.36 (6.45)</v>
+        <f t="shared" si="6"/>
+        <v>8.99 (0.28)</v>
       </c>
       <c r="K41" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>7.53 (0.23)</v>
+        <f t="shared" si="7"/>
+        <v>6.63 (0.21)</v>
       </c>
       <c r="L41" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>54</v>
-      </c>
+    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>27</v>
+        <v>220</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D42" s="1">
+        <v>65536</v>
       </c>
       <c r="E42" s="2">
-        <v>153.02000000000001</v>
+        <v>8.6881000000000004</v>
       </c>
       <c r="F42" s="2">
-        <v>101.62</v>
+        <v>57.640999999999998</v>
       </c>
       <c r="G42" s="2">
-        <v>30.07</v>
+        <v>2.8466999999999998</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>153.02 (1.00)</v>
+        <f t="shared" ref="I42:I43" si="8">IF(E42="","",TEXT(E42, "0.00")&amp;" (1.00)")</f>
+        <v>8.69 (1.00)</v>
       </c>
       <c r="J42" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>101.62 (0.66)</v>
+        <f t="shared" ref="J42:J43" si="9">IF(F42="","",TEXT(F42,"0.00")&amp;" ("&amp;TEXT(F42/$E42,"0.00")&amp;")")</f>
+        <v>57.64 (6.63)</v>
       </c>
       <c r="K42" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>30.07 (0.20)</v>
+        <f t="shared" ref="K42:K43" si="10">IF(G42="","",TEXT(G42,"0.00")&amp;" ("&amp;TEXT(G42/$E42,"0.00")&amp;")")</f>
+        <v>2.85 (0.33)</v>
       </c>
       <c r="L42" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="L42:L43" si="11">IF(H42="","",TEXT(H42,"0.00")&amp;" ("&amp;TEXT(H42/$E42,"0.00")&amp;")")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D43" s="1" t="s">
-        <v>28</v>
+      <c r="D43" s="1">
+        <v>262144</v>
       </c>
       <c r="E43" s="2">
-        <v>170.8</v>
+        <v>33.066000000000003</v>
       </c>
       <c r="F43" s="2">
-        <v>120.63</v>
+        <v>213.36</v>
       </c>
       <c r="G43" s="2">
-        <v>27.529</v>
+        <v>7.5279999999999996</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>170.80 (1.00)</v>
+        <f t="shared" si="8"/>
+        <v>33.07 (1.00)</v>
       </c>
       <c r="J43" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>120.63 (0.71)</v>
+        <f t="shared" si="9"/>
+        <v>213.36 (6.45)</v>
       </c>
       <c r="K43" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>27.53 (0.16)</v>
+        <f t="shared" si="10"/>
+        <v>7.53 (0.23)</v>
       </c>
       <c r="L43" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
       <c r="D44" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E44" s="2">
-        <v>170.99</v>
+        <v>153.02000000000001</v>
       </c>
       <c r="F44" s="2">
-        <v>108.14</v>
+        <v>101.62</v>
       </c>
       <c r="G44" s="2">
-        <v>29.541</v>
+        <v>30.07</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="1" t="str">
-        <f t="shared" ref="I44:I53" si="8">IF(E44="","",TEXT(E44, "0.00")&amp;" (1.00)")</f>
-        <v>170.99 (1.00)</v>
+        <f t="shared" si="0"/>
+        <v>153.02 (1.00)</v>
       </c>
       <c r="J44" s="1" t="str">
-        <f t="shared" ref="J44:J53" si="9">IF(F44="","",TEXT(F44,"0.00")&amp;" ("&amp;TEXT(F44/$E44,"0.00")&amp;")")</f>
-        <v>108.14 (0.63)</v>
+        <f t="shared" si="6"/>
+        <v>101.62 (0.66)</v>
       </c>
       <c r="K44" s="1" t="str">
-        <f t="shared" ref="K44:L53" si="10">IF(G44="","",TEXT(G44,"0.00")&amp;" ("&amp;TEXT(G44/$E44,"0.00")&amp;")")</f>
-        <v>29.54 (0.17)</v>
+        <f t="shared" si="7"/>
+        <v>30.07 (0.20)</v>
       </c>
       <c r="L44" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2701,296 +2733,358 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" t="s">
-        <v>30</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E45" s="2">
-        <v>39.222999999999999</v>
+        <v>170.8</v>
       </c>
       <c r="F45" s="2">
-        <v>11.346</v>
+        <v>120.63</v>
       </c>
       <c r="G45" s="2">
-        <v>8.6453000000000007</v>
+        <v>27.529</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>39.22 (1.00)</v>
+        <f t="shared" si="0"/>
+        <v>170.80 (1.00)</v>
       </c>
       <c r="J45" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>11.35 (0.29)</v>
+        <f t="shared" si="6"/>
+        <v>120.63 (0.71)</v>
       </c>
       <c r="K45" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>8.65 (0.22)</v>
+        <f t="shared" si="7"/>
+        <v>27.53 (0.16)</v>
       </c>
       <c r="L45" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D46" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E46" s="2">
-        <v>46.274999999999999</v>
+        <v>170.99</v>
       </c>
       <c r="F46" s="2">
-        <v>11.959</v>
+        <v>108.14</v>
       </c>
       <c r="G46" s="2">
-        <v>9.67</v>
+        <v>29.541</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>46.28 (1.00)</v>
+        <f t="shared" ref="I46:I55" si="12">IF(E46="","",TEXT(E46, "0.00")&amp;" (1.00)")</f>
+        <v>170.99 (1.00)</v>
       </c>
       <c r="J46" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>11.96 (0.26)</v>
+        <f t="shared" ref="J46:J55" si="13">IF(F46="","",TEXT(F46,"0.00")&amp;" ("&amp;TEXT(F46/$E46,"0.00")&amp;")")</f>
+        <v>108.14 (0.63)</v>
       </c>
       <c r="K46" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>9.67 (0.21)</v>
+        <f t="shared" ref="K46:L55" si="14">IF(G46="","",TEXT(G46,"0.00")&amp;" ("&amp;TEXT(G46/$E46,"0.00")&amp;")")</f>
+        <v>29.54 (0.17)</v>
       </c>
       <c r="L46" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
       <c r="D47" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E47" s="2">
-        <v>40.976999999999997</v>
+        <v>39.222999999999999</v>
       </c>
       <c r="F47" s="2">
-        <v>7.9154999999999998</v>
+        <v>11.346</v>
       </c>
       <c r="G47" s="2">
-        <v>8</v>
+        <v>8.6453000000000007</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>40.98 (1.00)</v>
+        <f t="shared" si="12"/>
+        <v>39.22 (1.00)</v>
       </c>
       <c r="J47" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>7.92 (0.19)</v>
+        <f t="shared" si="13"/>
+        <v>11.35 (0.29)</v>
       </c>
       <c r="K47" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>8.00 (0.20)</v>
+        <f t="shared" si="14"/>
+        <v>8.65 (0.22)</v>
       </c>
       <c r="L47" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" t="s">
-        <v>33</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E48" s="2">
-        <v>2.4849000000000001</v>
+        <v>46.274999999999999</v>
       </c>
       <c r="F48" s="2">
-        <v>8.2228999999999992</v>
+        <v>11.959</v>
       </c>
       <c r="G48" s="2">
-        <v>1.1926000000000001</v>
+        <v>9.67</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>2.48 (1.00)</v>
+        <f t="shared" si="12"/>
+        <v>46.28 (1.00)</v>
       </c>
       <c r="J48" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>8.22 (3.31)</v>
+        <f t="shared" si="13"/>
+        <v>11.96 (0.26)</v>
       </c>
       <c r="K48" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>1.19 (0.48)</v>
+        <f t="shared" si="14"/>
+        <v>9.67 (0.21)</v>
       </c>
       <c r="L48" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D49" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E49" s="2">
-        <v>2.5051000000000001</v>
+        <v>40.976999999999997</v>
       </c>
       <c r="F49" s="2">
-        <v>12.153</v>
+        <v>7.9154999999999998</v>
       </c>
       <c r="G49" s="2">
-        <v>1.2394000000000001</v>
+        <v>8</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>2.51 (1.00)</v>
+        <f t="shared" si="12"/>
+        <v>40.98 (1.00)</v>
       </c>
       <c r="J49" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>12.15 (4.85)</v>
+        <f t="shared" si="13"/>
+        <v>7.92 (0.19)</v>
       </c>
       <c r="K49" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>1.24 (0.49)</v>
+        <f t="shared" si="14"/>
+        <v>8.00 (0.20)</v>
       </c>
       <c r="L49" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
       <c r="D50" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E50" s="2">
-        <v>2.6457999999999999</v>
+        <v>2.4849000000000001</v>
       </c>
       <c r="F50" s="2">
-        <v>12.824999999999999</v>
+        <v>8.2228999999999992</v>
       </c>
       <c r="G50" s="2">
-        <v>1.2027000000000001</v>
+        <v>1.1926000000000001</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>2.65 (1.00)</v>
+        <f t="shared" si="12"/>
+        <v>2.48 (1.00)</v>
       </c>
       <c r="J50" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>12.83 (4.85)</v>
+        <f t="shared" si="13"/>
+        <v>8.22 (3.31)</v>
       </c>
       <c r="K50" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>1.20 (0.45)</v>
+        <f t="shared" si="14"/>
+        <v>1.19 (0.48)</v>
       </c>
       <c r="L50" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>230</v>
-      </c>
-      <c r="C51" t="s">
-        <v>231</v>
-      </c>
       <c r="D51" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E51" s="2">
-        <v>39.171999999999997</v>
+        <v>2.5051000000000001</v>
       </c>
       <c r="F51" s="2">
-        <v>54.83</v>
+        <v>12.153</v>
       </c>
       <c r="G51" s="2">
-        <v>11.946</v>
-      </c>
+        <v>1.2394000000000001</v>
+      </c>
+      <c r="H51" s="2"/>
       <c r="I51" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>39.17 (1.00)</v>
+        <f t="shared" si="12"/>
+        <v>2.51 (1.00)</v>
       </c>
       <c r="J51" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>54.83 (1.40)</v>
+        <f t="shared" si="13"/>
+        <v>12.15 (4.85)</v>
       </c>
       <c r="K51" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>11.95 (0.30)</v>
+        <f t="shared" si="14"/>
+        <v>1.24 (0.49)</v>
       </c>
       <c r="L51" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="2">
+        <v>2.6457999999999999</v>
+      </c>
+      <c r="F52" s="2">
+        <v>12.824999999999999</v>
+      </c>
+      <c r="G52" s="2">
+        <v>1.2027000000000001</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>2.65 (1.00)</v>
+      </c>
+      <c r="J52" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>12.83 (4.85)</v>
+      </c>
+      <c r="K52" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>1.20 (0.45)</v>
+      </c>
+      <c r="L52" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>230</v>
+      </c>
+      <c r="C53" t="s">
+        <v>231</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="2">
+        <v>39.171999999999997</v>
+      </c>
+      <c r="F53" s="2">
+        <v>54.83</v>
+      </c>
+      <c r="G53" s="2">
+        <v>11.946</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>39.17 (1.00)</v>
+      </c>
+      <c r="J53" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>54.83 (1.40)</v>
+      </c>
+      <c r="K53" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>11.95 (0.30)</v>
+      </c>
+      <c r="L53" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E54" s="2">
         <v>44.533000000000001</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F54" s="2">
         <v>55.308</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G54" s="2">
         <v>11.776999999999999</v>
       </c>
-      <c r="I52" s="1" t="str">
-        <f t="shared" si="8"/>
+      <c r="I54" s="1" t="str">
+        <f t="shared" si="12"/>
         <v>44.53 (1.00)</v>
       </c>
-      <c r="J52" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="J54" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>55.31 (1.24)</v>
       </c>
-      <c r="K52" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="K54" s="1" t="str">
+        <f t="shared" si="14"/>
         <v>11.78 (0.26)</v>
       </c>
-      <c r="L52" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="L54" s="1" t="str">
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D53" s="1" t="s">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D55" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E55" s="2">
         <v>41.22</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F55" s="2">
         <v>50.587000000000003</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G55" s="2">
         <v>11.467000000000001</v>
       </c>
-      <c r="I53" s="1" t="str">
-        <f t="shared" si="8"/>
+      <c r="I55" s="1" t="str">
+        <f t="shared" si="12"/>
         <v>41.22 (1.00)</v>
       </c>
-      <c r="J53" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="J55" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>50.59 (1.23)</v>
       </c>
-      <c r="K53" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="K55" s="1" t="str">
+        <f t="shared" si="14"/>
         <v>11.47 (0.28)</v>
       </c>
-      <c r="L53" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="L55" s="1" t="str">
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -3001,15 +3095,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD6D5CC-12E7-4025-9415-A12E1BCA77C3}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="7" width="15.5546875" customWidth="1"/>
@@ -3071,7 +3165,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B8" si="0">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A3&amp;")"</f>
+        <f t="shared" ref="B3:B9" si="0">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A3&amp;")"</f>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/collect_filtermap.rs)</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -3090,7 +3184,7 @@
         <v>168</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="G3:I8" si="1">"**"&amp;G3&amp;"**"</f>
+        <f t="shared" ref="I3:I9" si="1">"**"&amp;G3&amp;"**"</f>
         <v>****6.37 (0.40)****</v>
       </c>
     </row>
@@ -3152,84 +3246,112 @@
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" ref="B6" si="2">"[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/"&amp;A6&amp;")"</f>
+        <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/drain_vec_collect_map_filter.rs)</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ref="I6" si="3">"**"&amp;G6&amp;"**"</f>
+        <v>****12.84 (0.22)****</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/collect_map.rs)</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I6" t="str">
+      <c r="I7" t="str">
         <f t="shared" si="1"/>
         <v>****14.47 (0.40)****</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/collect_long_chain.rs)</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I7" t="str">
+      <c r="I8" t="str">
         <f t="shared" si="1"/>
         <v>****6.99 (0.19)****</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>214</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>[⇨](https://github.com/orxfun/orx-parallel/blob/main/benches/collect_iter_into_par.rs)</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>216</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>217</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>218</v>
       </c>
-      <c r="I8" t="str">
+      <c r="I9" t="str">
         <f t="shared" si="1"/>
         <v>****16.21 (0.34)****</v>
       </c>
@@ -4092,8 +4214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86143C3F-8878-42FB-956C-4C6FDD5D34D0}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>